<commit_message>
Update database for nations table
</commit_message>
<xml_diff>
--- a/public/template-personalinformation.xlsx
+++ b/public/template-personalinformation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Capstone\Doc\Assigned Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalVLU\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{17E09966-DC63-4F97-B342-B64D21BA71D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin nhân viên" sheetId="1" r:id="rId1"/>
@@ -20,11 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -176,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,8 +219,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -535,11 +531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,8 +722,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
+    <hyperlink ref="M3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -738,11 +734,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update unit test and update import function
</commit_message>
<xml_diff>
--- a/public/template-personalinformation.xlsx
+++ b/public/template-personalinformation.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PortalVLU\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\PortalVLU\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E631C3FC-CFA6-4A21-9F8F-A6D1CEF88639}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin nhân viên" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>Mã NV</t>
   </si>
@@ -176,12 +175,21 @@
   </si>
   <si>
     <t>Nhân sự</t>
+  </si>
+  <si>
+    <t>Chuyên Ngành</t>
+  </si>
+  <si>
+    <t>Công Nghệ Thông Tin</t>
+  </si>
+  <si>
+    <t>Quản Trị Kinh Doanh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,8 +236,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,11 +548,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,8 +748,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M3" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -752,120 +760,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1">
         <v>43200</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1">
         <v>43441</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1">
         <v>43388</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="1">
         <v>43388</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1">
         <v>43388</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>40</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add supervisor role , update model
add new role in admin ( only read data)

create new model and migrate update database
</commit_message>
<xml_diff>
--- a/public/template-personalinformation.xlsx
+++ b/public/template-personalinformation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>Mã NV</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Đơn vị</t>
   </si>
   <si>
-    <t>Hành chính</t>
-  </si>
-  <si>
     <t>Khối ngành</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Khối Ngành IV</t>
   </si>
   <si>
-    <t>Nhân sự</t>
-  </si>
-  <si>
     <t>Chuyên Ngành</t>
   </si>
   <si>
@@ -184,6 +178,9 @@
   </si>
   <si>
     <t>Quản Trị Kinh Doanh</t>
+  </si>
+  <si>
+    <t>Quan Hệ Công Chúng</t>
   </si>
 </sst>
 </file>
@@ -551,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +684,7 @@
         <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -743,7 +740,7 @@
         <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +781,7 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
@@ -793,7 +790,7 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,7 +801,7 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1">
         <v>43200</v>
@@ -813,7 +810,7 @@
         <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -824,7 +821,7 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1">
         <v>43441</v>
@@ -833,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -844,7 +841,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1">
         <v>43388</v>
@@ -853,7 +850,7 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,7 +861,7 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1">
         <v>43388</v>
@@ -873,7 +870,7 @@
         <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,7 +881,7 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1">
         <v>43388</v>
@@ -893,7 +890,7 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template pi for import
</commit_message>
<xml_diff>
--- a/public/template-personalinformation.xlsx
+++ b/public/template-personalinformation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin nhân viên" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
   <si>
     <t>Mã NV</t>
   </si>
@@ -412,6 +412,21 @@
   </si>
   <si>
     <t>Trung An 2</t>
+  </si>
+  <si>
+    <t>Trưởng phòng</t>
+  </si>
+  <si>
+    <t>Trưởng Khoa</t>
+  </si>
+  <si>
+    <t>Phó trưởng phòng</t>
+  </si>
+  <si>
+    <t>dsadsa</t>
+  </si>
+  <si>
+    <t>Loại cán sự</t>
   </si>
 </sst>
 </file>
@@ -492,7 +507,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -504,12 +519,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -540,6 +549,15 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -856,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,86 +903,90 @@
     <col min="23" max="23" width="20.7109375" customWidth="1"/>
     <col min="24" max="24" width="19.42578125" customWidth="1"/>
     <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:26" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1040,8 +1062,11 @@
       <c r="Y2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1106,7 +1131,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1171,7 +1196,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1230,8 +1255,11 @@
         <v>72</v>
       </c>
       <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -1295,8 +1323,11 @@
       <c r="V6" s="1">
         <v>43479</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1368,6 +1399,9 @@
       </c>
       <c r="X7" t="s">
         <v>49</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1423,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,28 +1438,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1634,19 +1668,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1693,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,50 +1746,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1770,7 +1804,7 @@
         <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
litte bug not expected
</commit_message>
<xml_diff>
--- a/public/template-personalinformation.xlsx
+++ b/public/template-personalinformation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\PortalVLU\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="thông tin nhân viên" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="131">
   <si>
     <t>Mã NV</t>
   </si>
@@ -387,9 +387,6 @@
     <t>Tôn giáo</t>
   </si>
   <si>
-    <t>Phật giáo</t>
-  </si>
-  <si>
     <t>Hòa hảo</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
   </si>
   <si>
     <t>Phó trưởng phòng</t>
-  </si>
-  <si>
-    <t>dsadsa</t>
   </si>
   <si>
     <t>Loại cán sự</t>
@@ -550,14 +544,14 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -877,7 +871,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,8 +976,8 @@
       <c r="Y1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="22" t="s">
-        <v>132</v>
+      <c r="Z1" s="20" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -1063,7 +1057,7 @@
         <v>49</v>
       </c>
       <c r="Z2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -1256,7 +1250,7 @@
       </c>
       <c r="V5" s="1"/>
       <c r="Z5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -1324,7 +1318,7 @@
         <v>43479</v>
       </c>
       <c r="Z6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -1401,7 +1395,7 @@
         <v>49</v>
       </c>
       <c r="Z7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1728,7 +1722,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,28 +1740,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
         <v>114</v>
       </c>
@@ -1801,25 +1795,25 @@
         <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J3" t="s">
         <v>16</v>
@@ -1830,28 +1824,28 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
         <v>122</v>
-      </c>
-      <c r="E4" t="s">
-        <v>123</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
fix redirect to 404 page after validate
</commit_message>
<xml_diff>
--- a/public/template-personalinformation.xlsx
+++ b/public/template-personalinformation.xlsx
@@ -195,7 +195,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Nhập " x " nếu nhân viên đó đã nghĩ hưu.</t>
+Nhập " x " nếu nhân viên đó đã nghĩ hưu hoặc bỏ trống nếu chưa nghĩ hưu</t>
         </r>
       </text>
     </comment>
@@ -305,16 +305,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Admin:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Có thể bỏ trống nếu người đó không phải là cán sự
 Danh sách loại cán sự:
 -Trưởng khoa
 -Phó Trưởng khoa
@@ -495,7 +496,16 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Có thể bỏ trống nếu cột Mã NV không có giá trị.</t>
+Có thể bỏ trống nếu cột Mã NV không có giá trị.
+Các loại khối ngành:
+-Khối ngành I
+-Khối ngành II
+-Khối ngành III
+-Khối ngành IV
+-Khối ngành V
+-Khối ngành VI
+-Khối ngành VII
+</t>
         </r>
       </text>
     </comment>
@@ -504,7 +514,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
   <si>
     <t>Mã NV</t>
   </si>
@@ -629,9 +639,6 @@
     <t>Trần Xuân Soạn</t>
   </si>
   <si>
-    <t>Loại hợp đồng</t>
-  </si>
-  <si>
     <t>Hợp đồng lao động</t>
   </si>
   <si>
@@ -741,6 +748,12 @@
   </si>
   <si>
     <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>Loại hợp đồng*</t>
+  </si>
+  <si>
+    <t>Khi có gặp lỗi những dòng đã xóa rồi mà vẫn hiển thị trên trang web, vui lòng chọn những dòng bị lỗi và sử dụng "Delete row(s)" trên thanh công cụ mục Cells trong tab Home</t>
   </si>
 </sst>
 </file>
@@ -750,7 +763,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -794,13 +807,26 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -831,7 +857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -882,6 +908,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1202,7 +1231,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,55 +1264,55 @@
   <sheetData>
     <row r="1" spans="1:27" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>61</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>7</v>
@@ -1313,7 +1342,7 @@
         <v>26</v>
       </c>
       <c r="AA1" s="18" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -1321,7 +1350,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1384,7 +1413,7 @@
         <v>14</v>
       </c>
       <c r="AA2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1418,28 +1447,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,7 +1535,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>6</v>
@@ -1539,16 +1568,16 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1">
         <v>43291</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1562,7 +1591,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:XFD2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,19 +1610,19 @@
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
@@ -1603,28 +1632,28 @@
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="H2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1672,14 +1701,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>